<commit_message>
created test Form Validation Mobile added new Stepdefinition updated Metadata file
</commit_message>
<xml_diff>
--- a/framework/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
+++ b/framework/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22568" windowHeight="9487" activeTab="3"/>
+    <workbookView windowWidth="22568" windowHeight="9487" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -183,10 +183,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -220,14 +220,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -242,14 +242,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -263,39 +255,63 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -310,6 +326,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -318,38 +349,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -364,25 +364,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -394,157 +544,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -571,17 +571,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -595,22 +589,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -630,17 +634,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -662,155 +660,157 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1291,8 +1291,8 @@
   <sheetPr/>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="7" outlineLevelCol="2"/>
@@ -1509,7 +1509,7 @@
   <sheetPr/>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
removed Staging env credentials; amended CPQ test with valid  workflow and instance for UAT
</commit_message>
<xml_diff>
--- a/framework/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
+++ b/framework/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22568" windowHeight="9487" activeTab="1"/>
+    <workbookView windowWidth="22568" windowHeight="10939"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="121">
   <si>
     <t>Tag</t>
   </si>
@@ -79,6 +79,129 @@
     <t>12space34</t>
   </si>
   <si>
+    <t>BUILDEMPIREADMINUSER</t>
+  </si>
+  <si>
+    <t>apprenticeships@bpptest.com</t>
+  </si>
+  <si>
+    <t>BUILDEMPIREADMINPASSWORD</t>
+  </si>
+  <si>
+    <t>Test Password003!</t>
+  </si>
+  <si>
+    <t>BUILDEMPIREMANAGERINUSER</t>
+  </si>
+  <si>
+    <t>waltdisney@mailinator.com</t>
+  </si>
+  <si>
+    <t>BUILDEMPIREMANAGERPASSWORD</t>
+  </si>
+  <si>
+    <t>Testing WALT 2018</t>
+  </si>
+  <si>
+    <t>BUILDEMPIRENEILADMINUSER</t>
+  </si>
+  <si>
+    <t>neilsteward@outlook.com</t>
+  </si>
+  <si>
+    <t>BUILDEMPIRENEILADMINPASSWORD</t>
+  </si>
+  <si>
+    <t>I am really really bored now!!</t>
+  </si>
+  <si>
+    <t>VLENOAHSTUDENTONE</t>
+  </si>
+  <si>
+    <t>student081601</t>
+  </si>
+  <si>
+    <t>VLENOAHTEACHERONE</t>
+  </si>
+  <si>
+    <t>teacher081602</t>
+  </si>
+  <si>
+    <t>VLENOAHPASS</t>
+  </si>
+  <si>
+    <t>Welcome1!</t>
+  </si>
+  <si>
+    <t>VLENOAHSTUDENTTWO</t>
+  </si>
+  <si>
+    <t>student081603</t>
+  </si>
+  <si>
+    <t>OPENBRAVOADMIN</t>
+  </si>
+  <si>
+    <t>ApolloAdminUAT</t>
+  </si>
+  <si>
+    <t>OPENBRAVOADMINPASSWORD</t>
+  </si>
+  <si>
+    <t>BUILDEMPIREVLESTUDENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">navigation@bpptest.com </t>
+  </si>
+  <si>
+    <t>BUILDEMPIREVLESTUDENTPASSWORD</t>
+  </si>
+  <si>
+    <t>Password TEST 2018</t>
+  </si>
+  <si>
+    <t>BARCLEYCARDACCOUNT</t>
+  </si>
+  <si>
+    <t>BPPProfEdLtd</t>
+  </si>
+  <si>
+    <t>BARCLEYCARDUSERNAME</t>
+  </si>
+  <si>
+    <t>Utopia</t>
+  </si>
+  <si>
+    <t>BARCLEYCARDPASSWORD</t>
+  </si>
+  <si>
+    <t>TestU2019Upd</t>
+  </si>
+  <si>
+    <t>ADMINISTRATEADMINUSERNAME</t>
+  </si>
+  <si>
+    <t>VolodymyrVeiko@bpp.com</t>
+  </si>
+  <si>
+    <t>ADMINISTRATEADMINPASSWORD</t>
+  </si>
+  <si>
+    <t>Liberty2015</t>
+  </si>
+  <si>
+    <t>TOTARAADMINUSER</t>
+  </si>
+  <si>
+    <t>bppadminnew@bpp.com</t>
+  </si>
+  <si>
+    <t>TOTARAADMINPASSWORD</t>
+  </si>
+  <si>
+    <t>Test Password001!</t>
+  </si>
+  <si>
     <t>ENTER</t>
   </si>
   <si>
@@ -142,7 +265,67 @@
     <t>SALESFORCEINSTANCE</t>
   </si>
   <si>
-    <t>https://bpp-13fd3e55182--noahuat.lightning.force.com/lightning/r/Instance__c/a5Cg0000000RXCcEAO/view</t>
+    <t>https://bpp-13fd3e55182--noahuat.lightning.force.com/lightning/r/Instance__c/a5Cg0000000ZaxTEAS/view</t>
+  </si>
+  <si>
+    <t>BUILDEMPIREBESPOKEURL</t>
+  </si>
+  <si>
+    <t>https://web-stage-bppdigital.bppuniversity.com/account?registration_type=rbs</t>
+  </si>
+  <si>
+    <t>BUILDEMPIRELOGINURL</t>
+  </si>
+  <si>
+    <t>https://web-stage-bppdigital.bppuniversity.com/account</t>
+  </si>
+  <si>
+    <t>BUILDEMPIRECHANNELISLANDURL</t>
+  </si>
+  <si>
+    <t>https://web-stage-bppdigital.bppuniversity.com/account?registration_type=jersey</t>
+  </si>
+  <si>
+    <t>BPPDIGITALINSIGHTSURL</t>
+  </si>
+  <si>
+    <t>https://web-stage-bppdigital.bppuniversity.com/insights</t>
+  </si>
+  <si>
+    <t>BPPDIGITALINDEXURL</t>
+  </si>
+  <si>
+    <t>https://web-stage-bppdigital.bppuniversity.com</t>
+  </si>
+  <si>
+    <t>BPPPDTESTCOURSEURL</t>
+  </si>
+  <si>
+    <t>https://web-stage-bppdigital.bppuniversity.com/courses/accountancy/test-automation</t>
+  </si>
+  <si>
+    <t>BPPBARCLEYCARDURL</t>
+  </si>
+  <si>
+    <t>https://ca-test.barclaycardsmartpay.com/ca/ca/login.shtml</t>
+  </si>
+  <si>
+    <t>BPPADMINISTRATEURL</t>
+  </si>
+  <si>
+    <t>https://bppsandbox.administrateapp.com</t>
+  </si>
+  <si>
+    <t>TOTARALOGINURL</t>
+  </si>
+  <si>
+    <t>https://totara-stage-bppdigital.bppuniversity.com</t>
+  </si>
+  <si>
+    <t>PDCOURSEURL</t>
+  </si>
+  <si>
+    <t>http://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/oksana-adm-course-1</t>
   </si>
   <si>
     <t>CUSTOMERGROUP</t>
@@ -163,19 +346,40 @@
     <t>SFCPQPRODUCT</t>
   </si>
   <si>
-    <t>SF CPQ test - SF CPQ test - SF CPQ flow test - London - In Centre - Classroom - AutoTest Sitting</t>
+    <t>CIMA - Operational Level - F1 Financial Reporting - Region 1 - Course Type 1 - QA 2021</t>
   </si>
   <si>
     <t>SFCPQINSTANCENUMBER</t>
   </si>
   <si>
-    <t>I-0942</t>
+    <t>I-2524</t>
   </si>
   <si>
     <t>CPQBOOKINGLINES</t>
   </si>
   <si>
     <t>(9)</t>
+  </si>
+  <si>
+    <t>CREDITCARDNUMBER</t>
+  </si>
+  <si>
+    <t>4111 1111 1111 1111</t>
+  </si>
+  <si>
+    <t>CREDITCARDHOLDERNAME</t>
+  </si>
+  <si>
+    <t>Adyen Test</t>
+  </si>
+  <si>
+    <t>CREDITCARDEXPIRYMONTH</t>
+  </si>
+  <si>
+    <t>CREDITCARDEXPIRYYEAR</t>
+  </si>
+  <si>
+    <t>CREDITCARDCVV</t>
   </si>
 </sst>
 </file>
@@ -183,9 +387,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
@@ -205,17 +409,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -226,8 +430,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -240,16 +469,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -262,9 +484,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -280,21 +501,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -302,14 +508,28 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -326,30 +546,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -364,103 +568,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -472,84 +748,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -558,24 +762,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color auto="1"/>
+        <color theme="4"/>
       </top>
-      <bottom/>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -604,6 +827,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -619,59 +851,18 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -689,132 +880,132 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -826,22 +1017,55 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -852,12 +1076,12 @@
     <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
     <cellStyle name="Currency" xfId="5" builtinId="4"/>
     <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
     <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
@@ -1162,18 +1386,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71559633027523" defaultRowHeight="14.5" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="33.8532110091743" style="6" customWidth="1"/>
-    <col min="2" max="2" width="45.4311926605505" style="6" customWidth="1"/>
-    <col min="3" max="3" width="44.1467889908257" style="6" customWidth="1"/>
-    <col min="4" max="16384" width="8.71559633027523" style="6"/>
+    <col min="1" max="1" width="33.8532110091743" style="15" customWidth="1"/>
+    <col min="2" max="2" width="45.4311926605505" style="15" customWidth="1"/>
+    <col min="3" max="3" width="44.1467889908257" style="15" customWidth="1"/>
+    <col min="4" max="16384" width="8.71559633027523" style="15"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:3">
@@ -1188,90 +1412,321 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="15" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" s="8" customFormat="1" spans="1:3">
-      <c r="A4" s="8" t="s">
+      <c r="C3" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" s="9" customFormat="1" spans="1:3">
+      <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" s="8" customFormat="1" spans="1:3">
-      <c r="A5" s="8" t="s">
+      <c r="C4" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" s="9" customFormat="1" spans="1:3">
+      <c r="A5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" s="8" customFormat="1" spans="1:3">
-      <c r="A6" s="8" t="s">
+      <c r="C5" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" s="9" customFormat="1" spans="1:3">
+      <c r="A6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" s="8" customFormat="1" spans="1:3">
-      <c r="A7" s="8" t="s">
+      <c r="C6" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" s="9" customFormat="1" spans="1:3">
+      <c r="A7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="13" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1279,6 +1734,10 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="automation@bpp.com.noahuat" tooltip="mailto:automation@bpp.com.noahuat"/>
     <hyperlink ref="B8" r:id="rId2" display="automationcpq@bpp.com.noahuat"/>
+    <hyperlink ref="B10" r:id="rId3" display="apprenticeships@bpptest.com"/>
+    <hyperlink ref="B12" r:id="rId4" display="waltdisney@mailinator.com"/>
+    <hyperlink ref="B14" r:id="rId5" display="neilsteward@outlook.com" tooltip="mailto:neilsteward@outlook.com"/>
+    <hyperlink ref="B29" r:id="rId6" display="bppadminnew@bpp.com"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>
@@ -1291,7 +1750,7 @@
   <sheetPr/>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -1315,10 +1774,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>20</v>
+        <v>61</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>61</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1326,10 +1785,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1337,10 +1796,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1348,10 +1807,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
@@ -1359,10 +1818,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
@@ -1370,10 +1829,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>5</v>
@@ -1381,10 +1840,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -1400,13 +1859,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="6" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
     <col min="2" max="2" width="140.43119266055" customWidth="1"/>
@@ -1425,11 +1884,11 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>31</v>
+      <c r="A2" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1437,10 +1896,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>33</v>
+        <v>73</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1448,45 +1907,155 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>35</v>
+        <v>75</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="8" t="s">
+      <c r="A5" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="8" t="s">
+      <c r="A6" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="8" t="s">
+      <c r="A7" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" s="16" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1496,7 +2065,16 @@
     <hyperlink ref="B3" r:id="rId2" display="https://vle-stage.bppuniversity.com/vle/login/index.php?authCAS=NOCAS" tooltip="https://vle-stage.bppuniversity.com/vle/login/index.php?authCAS=NOCAS"/>
     <hyperlink ref="B6" r:id="rId3" display="http://pprdbpp-sis-stage.apolloglobal.int/" tooltip="http://pprdbpp-sis-stage.apolloglobal.int/"/>
     <hyperlink ref="B4" r:id="rId4" display="https://login-stage.bppuniversity.com/ncas/login?service=https%3A%2F%2Fvle-stage.bppuniversity.com%2Fvle%2Flogin%2Findex.php%3FauthCAS%3DCAS" tooltip="https://login-stage.bppuniversity.com/ncas/login?service=https%3A%2F%2Fvle-stage.bppuniversity.com%2Fvle%2Flogin%2Findex.php%3FauthCAS%3DCAS"/>
-    <hyperlink ref="B7" r:id="rId5" display="https://bpp-13fd3e55182--noahuat.lightning.force.com/lightning/r/Instance__c/a5Cg0000000RXCcEAO/view"/>
+    <hyperlink ref="B7" r:id="rId5" display="https://bpp-13fd3e55182--noahuat.lightning.force.com/lightning/r/Instance__c/a5Cg0000000ZaxTEAS/view" tooltip="https://bpp-13fd3e55182--noahuat.lightning.force.com/lightning/r/Instance__c/a5Cg0000000ZaxTEAS/view"/>
+    <hyperlink ref="B9" r:id="rId6" display="https://web-stage-bppdigital.bppuniversity.com/account" tooltip="https://web-stage-bppdigital.bppuniversity.com/account"/>
+    <hyperlink ref="B10" r:id="rId7" display="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=jersey" tooltip="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=jersey"/>
+    <hyperlink ref="B8" r:id="rId8" display="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=rbs" tooltip="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=rbs"/>
+    <hyperlink ref="B16" r:id="rId9" display="https://totara-stage-bppdigital.bppuniversity.com" tooltip="https://totara-stage-bppdigital.bppuniversity.com"/>
+    <hyperlink ref="B17" r:id="rId10" display="http://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/oksana-adm-course-1" tooltip="http://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/oksana-adm-course-1"/>
+    <hyperlink ref="B12" r:id="rId11" display="https://web-stage-bppdigital.bppuniversity.com" tooltip="https://web-stage-bppdigital.bppuniversity.com"/>
+    <hyperlink ref="B13" r:id="rId12" display="https://web-stage-bppdigital.bppuniversity.com/courses/accountancy/test-automation"/>
+    <hyperlink ref="B11" r:id="rId13" display="https://web-stage-bppdigital.bppuniversity.com/insights" tooltip="https://web-stage-bppdigital.bppuniversity.com/insights"/>
+    <hyperlink ref="B15" r:id="rId14" display="https://bppsandbox.administrateapp.com"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>
@@ -1507,13 +2085,13 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B13" sqref="B9:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="6" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="26.7155963302752" customWidth="1"/>
     <col min="2" max="2" width="60.8256880733945" customWidth="1"/>
@@ -1533,10 +2111,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>103</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>104</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1544,10 +2122,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>44</v>
+        <v>105</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>45</v>
+        <v>106</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1555,7 +2133,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
       <c r="B4" s="2">
         <v>598587</v>
@@ -1566,10 +2144,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>48</v>
+        <v>109</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
@@ -1577,10 +2155,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>49</v>
+        <v>110</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>50</v>
+        <v>111</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
@@ -1588,12 +2166,78 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>51</v>
+        <v>112</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>52</v>
+        <v>113</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" s="5">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" s="5">
+        <v>2022</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" s="5">
+        <v>737</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
amended Direct Apps test for Academic Appeals; upgraded token
</commit_message>
<xml_diff>
--- a/framework/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
+++ b/framework/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="124">
   <si>
     <t>Tag</t>
   </si>
@@ -274,10 +274,19 @@
     <t>https://web-stage-bppdigital.bppuniversity.com/account?registration_type=rbs</t>
   </si>
   <si>
+    <t>BUILDEMPIREURL</t>
+  </si>
+  <si>
+    <t>https://web-stage-bppdigital.bppuniversity.com/account</t>
+  </si>
+  <si>
+    <t>BUILDEMPIREADMINURL</t>
+  </si>
+  <si>
+    <t>https://admin-stage-bppdigital.bppuniversity.com</t>
+  </si>
+  <si>
     <t>BUILDEMPIRELOGINURL</t>
-  </si>
-  <si>
-    <t>https://web-stage-bppdigital.bppuniversity.com/account</t>
   </si>
   <si>
     <t>BUILDEMPIRECHANNELISLANDURL</t>
@@ -387,12 +396,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,9 +424,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -431,39 +447,30 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -478,14 +485,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -501,6 +516,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -509,39 +532,24 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -553,7 +561,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -568,25 +584,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -598,13 +686,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -616,133 +740,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -762,28 +778,35 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -799,15 +822,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -836,33 +850,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -881,127 +897,127 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1026,9 +1042,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1042,12 +1055,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1056,9 +1075,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1389,7 +1405,7 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71559633027523" defaultRowHeight="14.5" outlineLevelCol="2"/>
@@ -1415,7 +1431,7 @@
       <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="20" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -1433,47 +1449,47 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" s="9" customFormat="1" spans="1:3">
-      <c r="A4" s="9" t="s">
+    <row r="4" s="8" customFormat="1" spans="1:3">
+      <c r="A4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" s="9" customFormat="1" spans="1:3">
-      <c r="A5" s="9" t="s">
+      <c r="C4" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" s="8" customFormat="1" spans="1:3">
+      <c r="A5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" s="9" customFormat="1" spans="1:3">
-      <c r="A6" s="9" t="s">
+      <c r="C5" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" s="8" customFormat="1" spans="1:3">
+      <c r="A6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" s="9" customFormat="1" spans="1:3">
-      <c r="A7" s="9" t="s">
+      <c r="C6" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" s="8" customFormat="1" spans="1:3">
+      <c r="A7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1481,10 +1497,10 @@
       <c r="A8" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1495,7 +1511,7 @@
       <c r="B9" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1503,7 +1519,7 @@
       <c r="A10" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="20" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="15" t="s">
@@ -1514,7 +1530,7 @@
       <c r="A11" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="15" t="s">
@@ -1525,7 +1541,7 @@
       <c r="A12" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="20" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="15" t="s">
@@ -1547,7 +1563,7 @@
       <c r="A14" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="20" t="s">
         <v>29</v>
       </c>
       <c r="C14" s="15" t="s">
@@ -1558,7 +1574,7 @@
       <c r="A15" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="15" t="s">
@@ -1569,7 +1585,7 @@
       <c r="A16" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C16" s="15" t="s">
@@ -1580,7 +1596,7 @@
       <c r="A17" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C17" s="15" t="s">
@@ -1591,7 +1607,7 @@
       <c r="A18" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="8" t="s">
         <v>37</v>
       </c>
       <c r="C18" s="15" t="s">
@@ -1599,134 +1615,134 @@
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="12" t="s">
         <v>43</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="12" t="s">
         <v>53</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="12" t="s">
         <v>57</v>
       </c>
       <c r="B29" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="12" t="s">
         <v>59</v>
       </c>
       <c r="B30" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="12" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1776,7 +1792,7 @@
       <c r="A2" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>61</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1859,10 +1875,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="2"/>
@@ -1920,10 +1936,10 @@
       <c r="A5" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1934,7 +1950,7 @@
       <c r="B6" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1942,26 +1958,26 @@
       <c r="A7" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="13" t="s">
         <v>85</v>
       </c>
       <c r="B9" s="14" t="s">
@@ -1972,90 +1988,112 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="15" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C11" s="16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="11" t="s">
+      <c r="B12" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="C12" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="C12" s="16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="11" t="s">
+      <c r="B13" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="C13" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="11" t="s">
+      <c r="B14" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="C14" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="11" t="s">
+      <c r="B15" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="C15" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="11" t="s">
+      <c r="B16" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="C16" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C16" s="16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="11" t="s">
+      <c r="B17" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="C17" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="B18" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" s="17" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2066,15 +2104,17 @@
     <hyperlink ref="B6" r:id="rId3" display="http://pprdbpp-sis-stage.apolloglobal.int/" tooltip="http://pprdbpp-sis-stage.apolloglobal.int/"/>
     <hyperlink ref="B4" r:id="rId4" display="https://login-stage.bppuniversity.com/ncas/login?service=https%3A%2F%2Fvle-stage.bppuniversity.com%2Fvle%2Flogin%2Findex.php%3FauthCAS%3DCAS" tooltip="https://login-stage.bppuniversity.com/ncas/login?service=https%3A%2F%2Fvle-stage.bppuniversity.com%2Fvle%2Flogin%2Findex.php%3FauthCAS%3DCAS"/>
     <hyperlink ref="B7" r:id="rId5" display="https://bpp-13fd3e55182--noahuat.lightning.force.com/lightning/r/Instance__c/a5Cg0000000ZaxTEAS/view" tooltip="https://bpp-13fd3e55182--noahuat.lightning.force.com/lightning/r/Instance__c/a5Cg0000000ZaxTEAS/view"/>
+    <hyperlink ref="B11" r:id="rId6" display="https://web-stage-bppdigital.bppuniversity.com/account" tooltip="https://web-stage-bppdigital.bppuniversity.com/account"/>
+    <hyperlink ref="B12" r:id="rId7" display="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=jersey" tooltip="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=jersey"/>
+    <hyperlink ref="B8" r:id="rId8" display="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=rbs" tooltip="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=rbs"/>
+    <hyperlink ref="B18" r:id="rId9" display="https://totara-stage-bppdigital.bppuniversity.com" tooltip="https://totara-stage-bppdigital.bppuniversity.com"/>
+    <hyperlink ref="B19" r:id="rId10" display="http://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/oksana-adm-course-1" tooltip="http://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/oksana-adm-course-1"/>
+    <hyperlink ref="B14" r:id="rId11" display="https://web-stage-bppdigital.bppuniversity.com" tooltip="https://web-stage-bppdigital.bppuniversity.com"/>
+    <hyperlink ref="B15" r:id="rId12" display="https://web-stage-bppdigital.bppuniversity.com/courses/accountancy/test-automation"/>
+    <hyperlink ref="B13" r:id="rId13" display="https://web-stage-bppdigital.bppuniversity.com/insights" tooltip="https://web-stage-bppdigital.bppuniversity.com/insights"/>
+    <hyperlink ref="B17" r:id="rId14" display="https://bppsandbox.administrateapp.com"/>
     <hyperlink ref="B9" r:id="rId6" display="https://web-stage-bppdigital.bppuniversity.com/account" tooltip="https://web-stage-bppdigital.bppuniversity.com/account"/>
-    <hyperlink ref="B10" r:id="rId7" display="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=jersey" tooltip="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=jersey"/>
-    <hyperlink ref="B8" r:id="rId8" display="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=rbs" tooltip="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=rbs"/>
-    <hyperlink ref="B16" r:id="rId9" display="https://totara-stage-bppdigital.bppuniversity.com" tooltip="https://totara-stage-bppdigital.bppuniversity.com"/>
-    <hyperlink ref="B17" r:id="rId10" display="http://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/oksana-adm-course-1" tooltip="http://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/oksana-adm-course-1"/>
-    <hyperlink ref="B12" r:id="rId11" display="https://web-stage-bppdigital.bppuniversity.com" tooltip="https://web-stage-bppdigital.bppuniversity.com"/>
-    <hyperlink ref="B13" r:id="rId12" display="https://web-stage-bppdigital.bppuniversity.com/courses/accountancy/test-automation"/>
-    <hyperlink ref="B11" r:id="rId13" display="https://web-stage-bppdigital.bppuniversity.com/insights" tooltip="https://web-stage-bppdigital.bppuniversity.com/insights"/>
-    <hyperlink ref="B15" r:id="rId14" display="https://bppsandbox.administrateapp.com"/>
+    <hyperlink ref="B10" r:id="rId15" display="https://admin-stage-bppdigital.bppuniversity.com" tooltip="https://admin-stage-bppdigital.bppuniversity.com"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>
@@ -2111,10 +2151,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -2122,10 +2162,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -2133,7 +2173,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B4" s="2">
         <v>598587</v>
@@ -2144,10 +2184,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
@@ -2155,10 +2195,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
@@ -2166,10 +2206,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>5</v>
@@ -2177,10 +2217,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -2188,10 +2228,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>5</v>
@@ -2199,10 +2239,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>5</v>
@@ -2210,7 +2250,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B11" s="5">
         <v>10</v>
@@ -2221,7 +2261,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B12" s="5">
         <v>2022</v>
@@ -2232,7 +2272,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B13" s="5">
         <v>737</v>

</xml_diff>

<commit_message>
added new tests for CPQ booking flow; amended Totara related tests; added new Step definitions; edited BE token and Metadata for Salesforce
</commit_message>
<xml_diff>
--- a/framework/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
+++ b/framework/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22568" windowHeight="10939"/>
+    <workbookView windowWidth="22568" windowHeight="9487" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="140">
   <si>
     <t>Tag</t>
   </si>
@@ -79,6 +79,24 @@
     <t>12space34</t>
   </si>
   <si>
+    <t>SALESFORCECSA</t>
+  </si>
+  <si>
+    <t>automationcsa@bpp.com.noahuat</t>
+  </si>
+  <si>
+    <t>SALESFORCECSAPASSWORD</t>
+  </si>
+  <si>
+    <t>SALESFORCESALES</t>
+  </si>
+  <si>
+    <t>automationsales@bpp.com.noahuat</t>
+  </si>
+  <si>
+    <t>SALESFORCESALESPASSWORD</t>
+  </si>
+  <si>
     <t>BUILDEMPIREADMINUSER</t>
   </si>
   <si>
@@ -268,6 +286,18 @@
     <t>https://bpp-13fd3e55182--noahuat.lightning.force.com/lightning/r/Instance__c/a5Cg0000000ZaxTEAS/view</t>
   </si>
   <si>
+    <t>SALESFORCESECONDINSTANCE</t>
+  </si>
+  <si>
+    <t>https://bpp-13fd3e55182--noahuat.lightning.force.com/lightning/r/Instance__c/a5Cg0000000ZbMuEAK/view</t>
+  </si>
+  <si>
+    <t>SALESFORCETHIRDINSTANCE</t>
+  </si>
+  <si>
+    <t>https://bpp-13fd3e55182--noahuat.lightning.force.com/lightning/r/Instance__c/a5Cg0000000ZbMzEAK/view</t>
+  </si>
+  <si>
     <t>BUILDEMPIREBESPOKEURL</t>
   </si>
   <si>
@@ -358,10 +388,28 @@
     <t>CIMA - Operational Level - F1 Financial Reporting - Region 1 - Course Type 1 - QA 2021</t>
   </si>
   <si>
+    <t>SFCPQPRODUCTSECOND</t>
+  </si>
+  <si>
+    <t>CIMA - Operational Level - null - Region 1 - Course Type 1 - QA 2021</t>
+  </si>
+  <si>
     <t>SFCPQINSTANCENUMBER</t>
   </si>
   <si>
     <t>I-2524</t>
+  </si>
+  <si>
+    <t>SFCPQSECONDINSTANCENUMBER</t>
+  </si>
+  <si>
+    <t>I-2916</t>
+  </si>
+  <si>
+    <t>SFCPQTHIRDINSTANCENUMBER</t>
+  </si>
+  <si>
+    <t>I-2917</t>
   </si>
   <si>
     <t>CPQBOOKINGLINES</t>
@@ -398,8 +446,8 @@
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -431,6 +479,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -440,7 +503,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -448,6 +526,37 @@
     <font>
       <b/>
       <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -462,30 +571,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -500,76 +617,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -584,13 +632,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -602,19 +662,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -626,31 +734,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -662,13 +794,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -680,91 +806,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -775,6 +823,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -798,54 +861,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -875,10 +890,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -896,128 +944,128 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1402,10 +1450,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71559633027523" defaultRowHeight="14.5" outlineLevelCol="2"/>
@@ -1522,7 +1570,7 @@
       <c r="B10" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1530,41 +1578,41 @@
       <c r="A11" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="15" t="s">
+      <c r="B11" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>5</v>
@@ -1572,10 +1620,10 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>5</v>
@@ -1583,10 +1631,10 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>31</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>5</v>
@@ -1594,10 +1642,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>33</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>5</v>
@@ -1605,65 +1653,65 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B19" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="12" t="s">
+      <c r="C19" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B20" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="12" t="s">
+      <c r="C20" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B21" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="12" t="s">
+      <c r="C21" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="12" t="s">
+      <c r="B22" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="15" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="13" t="s">
         <v>45</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>46</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>5</v>
@@ -1671,10 +1719,10 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="12" t="s">
         <v>47</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>48</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>5</v>
@@ -1682,10 +1730,10 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C25" s="12" t="s">
         <v>5</v>
@@ -1693,10 +1741,10 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>5</v>
@@ -1704,10 +1752,10 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>52</v>
       </c>
       <c r="C27" s="12" t="s">
         <v>5</v>
@@ -1715,10 +1763,10 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C28" s="12" t="s">
         <v>5</v>
@@ -1726,10 +1774,10 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B29" s="21" t="s">
-        <v>58</v>
+        <v>55</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>56</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>5</v>
@@ -1737,12 +1785,56 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="22" t="s">
+      <c r="B31" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C31" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" s="12" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1750,10 +1842,12 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="automation@bpp.com.noahuat" tooltip="mailto:automation@bpp.com.noahuat"/>
     <hyperlink ref="B8" r:id="rId2" display="automationcpq@bpp.com.noahuat"/>
-    <hyperlink ref="B10" r:id="rId3" display="apprenticeships@bpptest.com"/>
-    <hyperlink ref="B12" r:id="rId4" display="waltdisney@mailinator.com"/>
-    <hyperlink ref="B14" r:id="rId5" display="neilsteward@outlook.com" tooltip="mailto:neilsteward@outlook.com"/>
-    <hyperlink ref="B29" r:id="rId6" display="bppadminnew@bpp.com"/>
+    <hyperlink ref="B14" r:id="rId3" display="apprenticeships@bpptest.com"/>
+    <hyperlink ref="B16" r:id="rId4" display="waltdisney@mailinator.com"/>
+    <hyperlink ref="B18" r:id="rId5" display="neilsteward@outlook.com" tooltip="mailto:neilsteward@outlook.com"/>
+    <hyperlink ref="B33" r:id="rId6" display="bppadminnew@bpp.com"/>
+    <hyperlink ref="B10" r:id="rId7" display="automationcsa@bpp.com.noahuat"/>
+    <hyperlink ref="B12" r:id="rId8" display="automationsales@bpp.com.noahuat"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>
@@ -1790,10 +1884,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1801,10 +1895,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1812,10 +1906,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1823,10 +1917,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
@@ -1834,10 +1928,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
@@ -1845,10 +1939,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>5</v>
@@ -1856,10 +1950,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -1875,10 +1969,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="2"/>
@@ -1901,10 +1995,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1912,10 +2006,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1923,10 +2017,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1934,10 +2028,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="6" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>5</v>
@@ -1945,10 +2039,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="6" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>5</v>
@@ -1956,98 +2050,98 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="6" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="C8" s="12" t="s">
+      <c r="A8" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="C9" s="15" t="s">
+      <c r="A9" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="C10" s="15" t="s">
+      <c r="A10" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>86</v>
+      <c r="A11" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>96</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="C12" s="12" t="s">
+      <c r="A12" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" s="15" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="C13" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" s="15" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="10" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C14" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="10" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>5</v>
@@ -2055,10 +2149,10 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>99</v>
+        <v>104</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>105</v>
       </c>
       <c r="C16" s="17" t="s">
         <v>5</v>
@@ -2066,10 +2160,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="10" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>5</v>
@@ -2077,10 +2171,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>103</v>
+        <v>108</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>109</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>5</v>
@@ -2088,12 +2182,34 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="10" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C19" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C21" s="17" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2104,17 +2220,19 @@
     <hyperlink ref="B6" r:id="rId3" display="http://pprdbpp-sis-stage.apolloglobal.int/" tooltip="http://pprdbpp-sis-stage.apolloglobal.int/"/>
     <hyperlink ref="B4" r:id="rId4" display="https://login-stage.bppuniversity.com/ncas/login?service=https%3A%2F%2Fvle-stage.bppuniversity.com%2Fvle%2Flogin%2Findex.php%3FauthCAS%3DCAS" tooltip="https://login-stage.bppuniversity.com/ncas/login?service=https%3A%2F%2Fvle-stage.bppuniversity.com%2Fvle%2Flogin%2Findex.php%3FauthCAS%3DCAS"/>
     <hyperlink ref="B7" r:id="rId5" display="https://bpp-13fd3e55182--noahuat.lightning.force.com/lightning/r/Instance__c/a5Cg0000000ZaxTEAS/view" tooltip="https://bpp-13fd3e55182--noahuat.lightning.force.com/lightning/r/Instance__c/a5Cg0000000ZaxTEAS/view"/>
+    <hyperlink ref="B13" r:id="rId6" display="https://web-stage-bppdigital.bppuniversity.com/account" tooltip="https://web-stage-bppdigital.bppuniversity.com/account"/>
+    <hyperlink ref="B14" r:id="rId7" display="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=jersey" tooltip="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=jersey"/>
+    <hyperlink ref="B10" r:id="rId8" display="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=rbs" tooltip="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=rbs"/>
+    <hyperlink ref="B20" r:id="rId9" display="https://totara-stage-bppdigital.bppuniversity.com" tooltip="https://totara-stage-bppdigital.bppuniversity.com"/>
+    <hyperlink ref="B21" r:id="rId10" display="http://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/oksana-adm-course-1" tooltip="http://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/oksana-adm-course-1"/>
+    <hyperlink ref="B16" r:id="rId11" display="https://web-stage-bppdigital.bppuniversity.com" tooltip="https://web-stage-bppdigital.bppuniversity.com"/>
+    <hyperlink ref="B17" r:id="rId12" display="https://web-stage-bppdigital.bppuniversity.com/courses/accountancy/test-automation"/>
+    <hyperlink ref="B15" r:id="rId13" display="https://web-stage-bppdigital.bppuniversity.com/insights" tooltip="https://web-stage-bppdigital.bppuniversity.com/insights"/>
+    <hyperlink ref="B19" r:id="rId14" display="https://bppsandbox.administrateapp.com"/>
     <hyperlink ref="B11" r:id="rId6" display="https://web-stage-bppdigital.bppuniversity.com/account" tooltip="https://web-stage-bppdigital.bppuniversity.com/account"/>
-    <hyperlink ref="B12" r:id="rId7" display="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=jersey" tooltip="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=jersey"/>
-    <hyperlink ref="B8" r:id="rId8" display="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=rbs" tooltip="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=rbs"/>
-    <hyperlink ref="B18" r:id="rId9" display="https://totara-stage-bppdigital.bppuniversity.com" tooltip="https://totara-stage-bppdigital.bppuniversity.com"/>
-    <hyperlink ref="B19" r:id="rId10" display="http://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/oksana-adm-course-1" tooltip="http://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/oksana-adm-course-1"/>
-    <hyperlink ref="B14" r:id="rId11" display="https://web-stage-bppdigital.bppuniversity.com" tooltip="https://web-stage-bppdigital.bppuniversity.com"/>
-    <hyperlink ref="B15" r:id="rId12" display="https://web-stage-bppdigital.bppuniversity.com/courses/accountancy/test-automation"/>
-    <hyperlink ref="B13" r:id="rId13" display="https://web-stage-bppdigital.bppuniversity.com/insights" tooltip="https://web-stage-bppdigital.bppuniversity.com/insights"/>
-    <hyperlink ref="B17" r:id="rId14" display="https://bppsandbox.administrateapp.com"/>
-    <hyperlink ref="B9" r:id="rId6" display="https://web-stage-bppdigital.bppuniversity.com/account" tooltip="https://web-stage-bppdigital.bppuniversity.com/account"/>
-    <hyperlink ref="B10" r:id="rId15" display="https://admin-stage-bppdigital.bppuniversity.com" tooltip="https://admin-stage-bppdigital.bppuniversity.com"/>
+    <hyperlink ref="B12" r:id="rId15" display="https://admin-stage-bppdigital.bppuniversity.com" tooltip="https://admin-stage-bppdigital.bppuniversity.com"/>
+    <hyperlink ref="B8" r:id="rId16" display="https://bpp-13fd3e55182--noahuat.lightning.force.com/lightning/r/Instance__c/a5Cg0000000ZbMuEAK/view"/>
+    <hyperlink ref="B9" r:id="rId17" display="https://bpp-13fd3e55182--noahuat.lightning.force.com/lightning/r/Instance__c/a5Cg0000000ZbMzEAK/view"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>
@@ -2125,10 +2243,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B9:B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="2"/>
@@ -2151,10 +2269,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -2162,10 +2280,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -2173,7 +2291,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="B4" s="2">
         <v>598587</v>
@@ -2184,10 +2302,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
@@ -2195,10 +2313,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
@@ -2206,10 +2324,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>116</v>
+        <v>125</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>5</v>
@@ -2217,10 +2335,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -2228,10 +2346,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>118</v>
+        <v>129</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>130</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>5</v>
@@ -2239,10 +2357,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>120</v>
+        <v>131</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>5</v>
@@ -2250,10 +2368,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B11" s="5">
-        <v>10</v>
+        <v>116</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>5</v>
@@ -2261,10 +2379,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B12" s="5">
-        <v>2022</v>
+        <v>133</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>134</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>5</v>
@@ -2272,12 +2390,45 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B13" s="5">
+        <v>135</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14" s="5">
+        <v>10</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B15" s="5">
+        <v>2022</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B16" s="5">
         <v>737</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refactored Banner tests; edited product for CPQ flow updated tokens for BE and SF
</commit_message>
<xml_diff>
--- a/framework/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
+++ b/framework/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BPP\framework\src\main\resources\data\bpp\keywords.metadata\metadata\UAT\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86845E00-EB5C-4038-8866-0CD836319781}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="22568" windowHeight="9487" activeTab="3"/>
+    <workbookView xWindow="23125" yWindow="-109" windowWidth="23451" windowHeight="14134" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -17,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="139">
   <si>
     <t>Tag</t>
   </si>
@@ -389,9 +395,6 @@
   </si>
   <si>
     <t>SFCPQPRODUCTSECOND</t>
-  </si>
-  <si>
-    <t>CIMA - Operational Level - null - Region 1 - Course Type 1 - QA 2021</t>
   </si>
   <si>
     <t>SFCPQINSTANCENUMBER</t>
@@ -442,14 +445,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-  </numFmts>
-  <fonts count="23">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -479,36 +476,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -516,308 +483,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -825,249 +500,10 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1087,17 +523,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1106,13 +542,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1122,71 +558,28 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+  <cellStyles count="2">
+    <cellStyle name="Гіперпосилання" xfId="1" builtinId="8"/>
+    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1444,27 +837,27 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71559633027523" defaultRowHeight="14.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.55"/>
   <cols>
-    <col min="1" max="1" width="33.8532110091743" style="15" customWidth="1"/>
-    <col min="2" max="2" width="45.4311926605505" style="15" customWidth="1"/>
-    <col min="3" max="3" width="44.1467889908257" style="15" customWidth="1"/>
-    <col min="4" max="16384" width="8.71559633027523" style="15"/>
+    <col min="1" max="1" width="33.88671875" style="15" customWidth="1"/>
+    <col min="2" max="2" width="45.44140625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="44.109375" style="15" customWidth="1"/>
+    <col min="4" max="16384" width="8.6640625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:3">
+    <row r="1" spans="1:3" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1497,7 +890,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" s="8" customFormat="1" spans="1:3">
+    <row r="4" spans="1:3" s="8" customFormat="1">
       <c r="A4" s="8" t="s">
         <v>8</v>
       </c>
@@ -1508,7 +901,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" s="8" customFormat="1" spans="1:3">
+    <row r="5" spans="1:3" s="8" customFormat="1">
       <c r="A5" s="8" t="s">
         <v>10</v>
       </c>
@@ -1519,7 +912,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" s="8" customFormat="1" spans="1:3">
+    <row r="6" spans="1:3" s="8" customFormat="1">
       <c r="A6" s="8" t="s">
         <v>12</v>
       </c>
@@ -1530,7 +923,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" s="8" customFormat="1" spans="1:3">
+    <row r="7" spans="1:3" s="8" customFormat="1">
       <c r="A7" s="8" t="s">
         <v>14</v>
       </c>
@@ -1840,34 +1233,32 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="automation@bpp.com.noahuat" tooltip="mailto:automation@bpp.com.noahuat"/>
-    <hyperlink ref="B8" r:id="rId2" display="automationcpq@bpp.com.noahuat"/>
-    <hyperlink ref="B14" r:id="rId3" display="apprenticeships@bpptest.com"/>
-    <hyperlink ref="B16" r:id="rId4" display="waltdisney@mailinator.com"/>
-    <hyperlink ref="B18" r:id="rId5" display="neilsteward@outlook.com" tooltip="mailto:neilsteward@outlook.com"/>
-    <hyperlink ref="B33" r:id="rId6" display="bppadminnew@bpp.com"/>
-    <hyperlink ref="B10" r:id="rId7" display="automationcsa@bpp.com.noahuat"/>
-    <hyperlink ref="B12" r:id="rId8" display="automationsales@bpp.com.noahuat"/>
+    <hyperlink ref="B2" r:id="rId1" tooltip="mailto:automation@bpp.com.noahuat" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B8" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B14" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B16" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B18" r:id="rId5" tooltip="mailto:neilsteward@outlook.com" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B33" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
   </hyperlinks>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="7" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
   <cols>
-    <col min="1" max="1" width="16.7155963302752" customWidth="1"/>
-    <col min="2" max="2" width="26.7155963302752" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
     <col min="3" max="3" width="41" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1960,26 +1351,24 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="140.43119266055" customWidth="1"/>
-    <col min="3" max="3" width="26.1467889908257" customWidth="1"/>
+    <col min="2" max="2" width="140.44140625" customWidth="1"/>
+    <col min="3" max="3" width="26.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2215,45 +1604,43 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://cs21.salesforce.com/home/home.jsp"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://vle-stage.bppuniversity.com/vle/login/index.php?authCAS=NOCAS" tooltip="https://vle-stage.bppuniversity.com/vle/login/index.php?authCAS=NOCAS"/>
-    <hyperlink ref="B6" r:id="rId3" display="http://pprdbpp-sis-stage.apolloglobal.int/" tooltip="http://pprdbpp-sis-stage.apolloglobal.int/"/>
-    <hyperlink ref="B4" r:id="rId4" display="https://login-stage.bppuniversity.com/ncas/login?service=https%3A%2F%2Fvle-stage.bppuniversity.com%2Fvle%2Flogin%2Findex.php%3FauthCAS%3DCAS" tooltip="https://login-stage.bppuniversity.com/ncas/login?service=https%3A%2F%2Fvle-stage.bppuniversity.com%2Fvle%2Flogin%2Findex.php%3FauthCAS%3DCAS"/>
-    <hyperlink ref="B7" r:id="rId5" display="https://bpp-13fd3e55182--noahuat.lightning.force.com/lightning/r/Instance__c/a5Cg0000000ZaxTEAS/view" tooltip="https://bpp-13fd3e55182--noahuat.lightning.force.com/lightning/r/Instance__c/a5Cg0000000ZaxTEAS/view"/>
-    <hyperlink ref="B13" r:id="rId6" display="https://web-stage-bppdigital.bppuniversity.com/account" tooltip="https://web-stage-bppdigital.bppuniversity.com/account"/>
-    <hyperlink ref="B14" r:id="rId7" display="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=jersey" tooltip="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=jersey"/>
-    <hyperlink ref="B10" r:id="rId8" display="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=rbs" tooltip="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=rbs"/>
-    <hyperlink ref="B20" r:id="rId9" display="https://totara-stage-bppdigital.bppuniversity.com" tooltip="https://totara-stage-bppdigital.bppuniversity.com"/>
-    <hyperlink ref="B21" r:id="rId10" display="http://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/oksana-adm-course-1" tooltip="http://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/oksana-adm-course-1"/>
-    <hyperlink ref="B16" r:id="rId11" display="https://web-stage-bppdigital.bppuniversity.com" tooltip="https://web-stage-bppdigital.bppuniversity.com"/>
-    <hyperlink ref="B17" r:id="rId12" display="https://web-stage-bppdigital.bppuniversity.com/courses/accountancy/test-automation"/>
-    <hyperlink ref="B15" r:id="rId13" display="https://web-stage-bppdigital.bppuniversity.com/insights" tooltip="https://web-stage-bppdigital.bppuniversity.com/insights"/>
-    <hyperlink ref="B19" r:id="rId14" display="https://bppsandbox.administrateapp.com"/>
-    <hyperlink ref="B11" r:id="rId6" display="https://web-stage-bppdigital.bppuniversity.com/account" tooltip="https://web-stage-bppdigital.bppuniversity.com/account"/>
-    <hyperlink ref="B12" r:id="rId15" display="https://admin-stage-bppdigital.bppuniversity.com" tooltip="https://admin-stage-bppdigital.bppuniversity.com"/>
-    <hyperlink ref="B8" r:id="rId16" display="https://bpp-13fd3e55182--noahuat.lightning.force.com/lightning/r/Instance__c/a5Cg0000000ZbMuEAK/view"/>
-    <hyperlink ref="B9" r:id="rId17" display="https://bpp-13fd3e55182--noahuat.lightning.force.com/lightning/r/Instance__c/a5Cg0000000ZbMzEAK/view"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" tooltip="https://vle-stage.bppuniversity.com/vle/login/index.php?authCAS=NOCAS" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="B6" r:id="rId3" tooltip="http://pprdbpp-sis-stage.apolloglobal.int/" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="B4" r:id="rId4" tooltip="https://login-stage.bppuniversity.com/ncas/login?service=https%3A%2F%2Fvle-stage.bppuniversity.com%2Fvle%2Flogin%2Findex.php%3FauthCAS%3DCAS" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="B7" r:id="rId5" tooltip="https://bpp-13fd3e55182--noahuat.lightning.force.com/lightning/r/Instance__c/a5Cg0000000ZaxTEAS/view" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="B13" r:id="rId6" tooltip="https://web-stage-bppdigital.bppuniversity.com/account" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="B14" r:id="rId7" tooltip="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=jersey" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="B10" r:id="rId8" tooltip="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=rbs" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="B20" r:id="rId9" tooltip="https://totara-stage-bppdigital.bppuniversity.com" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="B21" r:id="rId10" tooltip="http://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/oksana-adm-course-1" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="B16" r:id="rId11" tooltip="https://web-stage-bppdigital.bppuniversity.com" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="B17" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="B15" r:id="rId13" tooltip="https://web-stage-bppdigital.bppuniversity.com/insights" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
+    <hyperlink ref="B19" r:id="rId14" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
+    <hyperlink ref="B11" r:id="rId15" tooltip="https://web-stage-bppdigital.bppuniversity.com/account" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
+    <hyperlink ref="B12" r:id="rId16" tooltip="https://admin-stage-bppdigital.bppuniversity.com" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
+    <hyperlink ref="B8" r:id="rId17" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
+    <hyperlink ref="B9" r:id="rId18" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
   </hyperlinks>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
   <cols>
-    <col min="1" max="1" width="26.7155963302752" customWidth="1"/>
-    <col min="2" max="2" width="60.8256880733945" customWidth="1"/>
-    <col min="3" max="3" width="37.7155963302752" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" customWidth="1"/>
+    <col min="2" max="2" width="67.77734375" customWidth="1"/>
+    <col min="3" max="3" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2316,7 +1703,7 @@
         <v>123</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
@@ -2324,10 +1711,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>126</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>5</v>
@@ -2335,10 +1722,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -2346,10 +1733,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>5</v>
@@ -2357,10 +1744,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>131</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>132</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>5</v>
@@ -2379,10 +1766,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>133</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>134</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>5</v>
@@ -2390,10 +1777,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>135</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>136</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>5</v>
@@ -2401,7 +1788,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B14" s="5">
         <v>10</v>
@@ -2412,7 +1799,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B15" s="5">
         <v>2022</v>
@@ -2423,7 +1810,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B16" s="5">
         <v>737</v>
@@ -2433,7 +1820,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Dates and Prices test created.
</commit_message>
<xml_diff>
--- a/framework/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
+++ b/framework/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruslan.levytskyi\IdeaProjects\qa-automation-framework-bdd\framework\src\main\resources\data\bpp\keywords.metadata\metadata\UAT\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5953EB07-DE1E-4640-96FF-9A8E34D572A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="22568" windowHeight="9487" activeTab="3"/>
+    <workbookView xWindow="1992" yWindow="120" windowWidth="20484" windowHeight="12360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -17,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="146">
   <si>
     <t>Tag</t>
   </si>
@@ -437,19 +443,31 @@
   </si>
   <si>
     <t>CREDITCARDCVV</t>
+  </si>
+  <si>
+    <t>https://uat-products.bpp.com/</t>
+  </si>
+  <si>
+    <t>PRODUCTFACTORYUSER</t>
+  </si>
+  <si>
+    <t>PRODUCTFACTORYPASSWORD</t>
+  </si>
+  <si>
+    <t>yuriizosin@bpp.com</t>
+  </si>
+  <si>
+    <t>Welcome9@</t>
+  </si>
+  <si>
+    <t>PRODUCTFACTORYURLNEW</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-  </numFmts>
-  <fonts count="23">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -479,36 +497,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -516,308 +504,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -825,251 +521,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1087,17 +544,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1106,13 +563,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1122,71 +579,34 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1444,27 +864,27 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:C34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71559633027523" defaultRowHeight="14.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="33.8532110091743" style="15" customWidth="1"/>
-    <col min="2" max="2" width="45.4311926605505" style="15" customWidth="1"/>
-    <col min="3" max="3" width="44.1467889908257" style="15" customWidth="1"/>
-    <col min="4" max="16384" width="8.71559633027523" style="15"/>
+    <col min="1" max="1" width="33.88671875" style="15" customWidth="1"/>
+    <col min="2" max="2" width="45.44140625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="44.109375" style="15" customWidth="1"/>
+    <col min="4" max="16384" width="8.6640625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:3">
+    <row r="1" spans="1:3" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1497,7 +917,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" s="8" customFormat="1" spans="1:3">
+    <row r="4" spans="1:3" s="8" customFormat="1">
       <c r="A4" s="8" t="s">
         <v>8</v>
       </c>
@@ -1508,7 +928,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" s="8" customFormat="1" spans="1:3">
+    <row r="5" spans="1:3" s="8" customFormat="1">
       <c r="A5" s="8" t="s">
         <v>10</v>
       </c>
@@ -1519,7 +939,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" s="8" customFormat="1" spans="1:3">
+    <row r="6" spans="1:3" s="8" customFormat="1">
       <c r="A6" s="8" t="s">
         <v>12</v>
       </c>
@@ -1530,7 +950,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" s="8" customFormat="1" spans="1:3">
+    <row r="7" spans="1:3" s="8" customFormat="1">
       <c r="A7" s="8" t="s">
         <v>14</v>
       </c>
@@ -1838,36 +1258,58 @@
         <v>5</v>
       </c>
     </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B35" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="B36" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="automation@bpp.com.noahuat" tooltip="mailto:automation@bpp.com.noahuat"/>
-    <hyperlink ref="B8" r:id="rId2" display="automationcpq@bpp.com.noahuat"/>
-    <hyperlink ref="B14" r:id="rId3" display="apprenticeships@bpptest.com"/>
-    <hyperlink ref="B16" r:id="rId4" display="waltdisney@mailinator.com"/>
-    <hyperlink ref="B18" r:id="rId5" display="neilsteward@outlook.com" tooltip="mailto:neilsteward@outlook.com"/>
-    <hyperlink ref="B33" r:id="rId6" display="bppadminnew@bpp.com"/>
-    <hyperlink ref="B10" r:id="rId7" display="automationcsa@bpp.com.noahuat"/>
-    <hyperlink ref="B12" r:id="rId8" display="automationsales@bpp.com.noahuat"/>
+    <hyperlink ref="B2" r:id="rId1" tooltip="mailto:automation@bpp.com.noahuat" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B8" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B14" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B16" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B18" r:id="rId5" tooltip="mailto:neilsteward@outlook.com" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B33" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B35" r:id="rId9" xr:uid="{ECCDA514-8F41-410A-B8AE-7A69060C22B2}"/>
+    <hyperlink ref="B36" r:id="rId10" xr:uid="{8FD7F45B-6133-4C22-915A-CDDDDB5344C1}"/>
   </hyperlinks>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="7" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.7155963302752" customWidth="1"/>
-    <col min="2" max="2" width="26.7155963302752" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
     <col min="3" max="3" width="41" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1960,26 +1402,24 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:C21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="140.43119266055" customWidth="1"/>
-    <col min="3" max="3" width="26.1467889908257" customWidth="1"/>
+    <col min="2" max="2" width="140.44140625" customWidth="1"/>
+    <col min="3" max="3" width="26.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2213,47 +1653,57 @@
         <v>5</v>
       </c>
     </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://cs21.salesforce.com/home/home.jsp"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://vle-stage.bppuniversity.com/vle/login/index.php?authCAS=NOCAS" tooltip="https://vle-stage.bppuniversity.com/vle/login/index.php?authCAS=NOCAS"/>
-    <hyperlink ref="B6" r:id="rId3" display="http://pprdbpp-sis-stage.apolloglobal.int/" tooltip="http://pprdbpp-sis-stage.apolloglobal.int/"/>
-    <hyperlink ref="B4" r:id="rId4" display="https://login-stage.bppuniversity.com/ncas/login?service=https%3A%2F%2Fvle-stage.bppuniversity.com%2Fvle%2Flogin%2Findex.php%3FauthCAS%3DCAS" tooltip="https://login-stage.bppuniversity.com/ncas/login?service=https%3A%2F%2Fvle-stage.bppuniversity.com%2Fvle%2Flogin%2Findex.php%3FauthCAS%3DCAS"/>
-    <hyperlink ref="B7" r:id="rId5" display="https://bpp-13fd3e55182--noahuat.lightning.force.com/lightning/r/Instance__c/a5Cg0000000ZaxTEAS/view" tooltip="https://bpp-13fd3e55182--noahuat.lightning.force.com/lightning/r/Instance__c/a5Cg0000000ZaxTEAS/view"/>
-    <hyperlink ref="B13" r:id="rId6" display="https://web-stage-bppdigital.bppuniversity.com/account" tooltip="https://web-stage-bppdigital.bppuniversity.com/account"/>
-    <hyperlink ref="B14" r:id="rId7" display="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=jersey" tooltip="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=jersey"/>
-    <hyperlink ref="B10" r:id="rId8" display="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=rbs" tooltip="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=rbs"/>
-    <hyperlink ref="B20" r:id="rId9" display="https://totara-stage-bppdigital.bppuniversity.com" tooltip="https://totara-stage-bppdigital.bppuniversity.com"/>
-    <hyperlink ref="B21" r:id="rId10" display="http://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/oksana-adm-course-1" tooltip="http://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/oksana-adm-course-1"/>
-    <hyperlink ref="B16" r:id="rId11" display="https://web-stage-bppdigital.bppuniversity.com" tooltip="https://web-stage-bppdigital.bppuniversity.com"/>
-    <hyperlink ref="B17" r:id="rId12" display="https://web-stage-bppdigital.bppuniversity.com/courses/accountancy/test-automation"/>
-    <hyperlink ref="B15" r:id="rId13" display="https://web-stage-bppdigital.bppuniversity.com/insights" tooltip="https://web-stage-bppdigital.bppuniversity.com/insights"/>
-    <hyperlink ref="B19" r:id="rId14" display="https://bppsandbox.administrateapp.com"/>
-    <hyperlink ref="B11" r:id="rId6" display="https://web-stage-bppdigital.bppuniversity.com/account" tooltip="https://web-stage-bppdigital.bppuniversity.com/account"/>
-    <hyperlink ref="B12" r:id="rId15" display="https://admin-stage-bppdigital.bppuniversity.com" tooltip="https://admin-stage-bppdigital.bppuniversity.com"/>
-    <hyperlink ref="B8" r:id="rId16" display="https://bpp-13fd3e55182--noahuat.lightning.force.com/lightning/r/Instance__c/a5Cg0000000ZbMuEAK/view"/>
-    <hyperlink ref="B9" r:id="rId17" display="https://bpp-13fd3e55182--noahuat.lightning.force.com/lightning/r/Instance__c/a5Cg0000000ZbMzEAK/view"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" tooltip="https://vle-stage.bppuniversity.com/vle/login/index.php?authCAS=NOCAS" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="B6" r:id="rId3" tooltip="http://pprdbpp-sis-stage.apolloglobal.int/" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="B4" r:id="rId4" tooltip="https://login-stage.bppuniversity.com/ncas/login?service=https%3A%2F%2Fvle-stage.bppuniversity.com%2Fvle%2Flogin%2Findex.php%3FauthCAS%3DCAS" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="B7" r:id="rId5" tooltip="https://bpp-13fd3e55182--noahuat.lightning.force.com/lightning/r/Instance__c/a5Cg0000000ZaxTEAS/view" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="B13" r:id="rId6" tooltip="https://web-stage-bppdigital.bppuniversity.com/account" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="B14" r:id="rId7" tooltip="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=jersey" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="B10" r:id="rId8" tooltip="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=rbs" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="B20" r:id="rId9" tooltip="https://totara-stage-bppdigital.bppuniversity.com" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="B21" r:id="rId10" tooltip="http://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/oksana-adm-course-1" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="B16" r:id="rId11" tooltip="https://web-stage-bppdigital.bppuniversity.com" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="B17" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="B15" r:id="rId13" tooltip="https://web-stage-bppdigital.bppuniversity.com/insights" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
+    <hyperlink ref="B19" r:id="rId14" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
+    <hyperlink ref="B11" r:id="rId15" tooltip="https://web-stage-bppdigital.bppuniversity.com/account" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
+    <hyperlink ref="B12" r:id="rId16" tooltip="https://admin-stage-bppdigital.bppuniversity.com" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
+    <hyperlink ref="B8" r:id="rId17" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
+    <hyperlink ref="B9" r:id="rId18" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
+    <hyperlink ref="B22" r:id="rId19" xr:uid="{ED23AE1F-B332-424F-B2C6-5374E4B9BE74}"/>
   </hyperlinks>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.7155963302752" customWidth="1"/>
-    <col min="2" max="2" width="60.8256880733945" customWidth="1"/>
-    <col min="3" max="3" width="37.7155963302752" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" customWidth="1"/>
+    <col min="2" max="2" width="60.77734375" customWidth="1"/>
+    <col min="3" max="3" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2433,7 +1883,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated CSA End to end test due to Yahoo captcha for login
</commit_message>
<xml_diff>
--- a/framework/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
+++ b/framework/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruslan.levytskyi\IdeaProjects\qa-automation-framework-bdd\framework\src\main\resources\data\bpp\keywords.metadata\metadata\UAT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BPP\framework\src\main\resources\data\bpp\keywords.metadata\metadata\UAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF8A7723-4C7C-4EE8-B192-3DEFFA2674E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04BC745B-9D4D-4765-AC49-516C056F97C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37350" yWindow="1230" windowWidth="16395" windowHeight="9885" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23125" yWindow="-109" windowWidth="23451" windowHeight="14134" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="149">
   <si>
     <t>Tag</t>
   </si>
@@ -458,18 +458,37 @@
   </si>
   <si>
     <t>https://uat-products.bpp.com/</t>
+  </si>
+  <si>
+    <t>YAHOOEMAILCASEUSER</t>
+  </si>
+  <si>
+    <t>YAHOOEMAILCASEPASSWORD</t>
+  </si>
+  <si>
+    <t>Casemail123</t>
+  </si>
+  <si>
+    <t>casemail777@yahoo.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -501,6 +520,12 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -521,11 +546,11 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -538,58 +563,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Гіперпосилання" xfId="1" builtinId="8"/>
+    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium7"/>
@@ -862,13 +896,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:C36"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.55"/>
   <cols>
     <col min="1" max="1" width="33.88671875" style="15" customWidth="1"/>
     <col min="2" max="2" width="45.44140625" style="15" customWidth="1"/>
@@ -913,7 +947,7 @@
       <c r="A4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="24" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="8" t="s">
@@ -1251,24 +1285,46 @@
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" t="s">
+      <c r="A35" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" t="s">
+      <c r="A36" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B36" s="23" t="s">
+      <c r="B36" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="B37" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="C38" s="15" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1283,9 +1339,11 @@
     <hyperlink ref="B10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="B12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="B36" r:id="rId9" xr:uid="{70F4196F-0B8A-4153-B91C-F4B4CC8EDD74}"/>
+    <hyperlink ref="B4" r:id="rId10" xr:uid="{916316F4-798F-403B-8DD7-03162CC48981}"/>
+    <hyperlink ref="B37" r:id="rId11" xr:uid="{964FCB21-86AC-430F-A7D7-AC890B429861}"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
 
@@ -1297,7 +1355,7 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
   <cols>
     <col min="1" max="1" width="16.6640625" customWidth="1"/>
     <col min="2" max="2" width="26.6640625" customWidth="1"/>
@@ -1402,11 +1460,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+    <sheetView topLeftCell="B13" workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
     <col min="2" max="2" width="140.44140625" customWidth="1"/>
@@ -1690,7 +1748,7 @@
       <selection activeCell="A17" sqref="A17:C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
   <cols>
     <col min="1" max="1" width="26.6640625" customWidth="1"/>
     <col min="2" max="2" width="67.77734375" customWidth="1"/>

</xml_diff>